<commit_message>
Replaced new ICs with versions in the oresat-eagle-libraries repo
</commit_message>
<xml_diff>
--- a/BOM/C3-Practicum.xlsx
+++ b/BOM/C3-Practicum.xlsx
@@ -562,7 +562,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD;@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -592,12 +592,6 @@
       <name val="Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -668,7 +662,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -725,10 +719,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -749,10 +739,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -765,20 +751,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -878,24 +856,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6383928571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7410714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3258928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2633928571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4107142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3705357142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,7 +1149,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1192,24 +1170,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6964285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1205357142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7410714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3258928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2633928571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4107142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4419642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1358,7 @@
       <c r="F9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -1440,7 +1418,7 @@
       <c r="F11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="7" t="s">
         <v>63</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -1454,66 +1432,66 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="n">
+      <c r="A12" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="7" t="s">
         <v>67</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="n">
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="7" t="s">
         <v>71</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="17" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1534,7 +1512,7 @@
       <c r="F14" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>77</v>
       </c>
       <c r="H14" s="7" t="s">
@@ -1577,414 +1555,414 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="n">
+    <row r="16" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="16" t="s">
         <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="n">
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="16" t="s">
         <v>92</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="n">
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="16" t="s">
         <v>96</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="n">
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="16" t="s">
         <v>101</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="n">
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="16" t="s">
         <v>106</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="n">
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="16" t="s">
         <v>111</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-    </row>
-    <row r="22" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="n">
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+    </row>
+    <row r="22" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="16" t="s">
         <v>115</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-    </row>
-    <row r="23" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="n">
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="16" t="s">
         <v>120</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-    </row>
-    <row r="24" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="n">
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="16" t="s">
         <v>123</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="J24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="n">
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+    </row>
+    <row r="25" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="16" t="s">
         <v>127</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="n">
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+    </row>
+    <row r="26" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-    </row>
-    <row r="27" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="n">
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+    </row>
+    <row r="27" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="J27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-    </row>
-    <row r="28" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="20"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="21"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+    </row>
+    <row r="29" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
@@ -2045,7 +2023,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2066,24 +2044,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6383928571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7410714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3258928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2633928571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4107142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,7 +2334,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2377,24 +2355,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3258928571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="25" width="12.6383928571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="25" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="25" width="37.3258928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="19" width="10.2767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2633928571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4107142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0892857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="12.4017857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="16.65625"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="18" width="10.0401785714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2399,7 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="0"/>
@@ -2440,7 +2418,7 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="0"/>
@@ -2502,13 +2480,13 @@
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="23" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -2540,16 +2518,16 @@
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="18" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="0" t="s">
@@ -2572,16 +2550,16 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="18" t="s">
         <v>145</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2601,16 +2579,16 @@
       <c r="D10" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I10" s="0" t="s">
@@ -2625,7 +2603,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="24" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -2634,16 +2612,16 @@
       <c r="D11" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I11" s="0" t="s">
@@ -2666,16 +2644,16 @@
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="0" t="s">
@@ -2698,16 +2676,16 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I13" s="0" t="s">
@@ -2716,16 +2694,26 @@
       <c r="J13" s="1" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="J14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="9"/>
       <c r="J15" s="8"/>
       <c r="K15" s="9"/>
@@ -2790,7 +2778,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2811,24 +2799,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.4732142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.62053571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6383928571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.7410714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.3258928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2767857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5669642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="36.2633928571429"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.5223214285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.4107142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.97767857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.2991071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.97767857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1205357142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2955,6 +2943,78 @@
       <c r="B8" s="0"/>
       <c r="D8" s="0"/>
       <c r="J8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="J9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="J10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="J11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="J12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="J13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="J14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="J15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="J16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="J17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="J18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="J19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="J20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
@@ -3013,7 +3073,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added the BOM for the practicum C3 board
</commit_message>
<xml_diff>
--- a/BOM/C3-Practicum.xlsx
+++ b/BOM/C3-Practicum.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="218">
   <si>
     <t xml:space="preserve">Bill Of Materials</t>
   </si>
@@ -167,10 +167,10 @@
     <t xml:space="preserve">oresat-c3-prototype</t>
   </si>
   <si>
-    <t xml:space="preserve">Modified: 2019-11-22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1,C5,C10,C14,</t>
+    <t xml:space="preserve">Modified: 2019-11-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1,4,5,10,20</t>
   </si>
   <si>
     <t xml:space="preserve">Yageo</t>
@@ -191,7 +191,7 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">C2,3,4,6,8,9,13,15,17,22</t>
+    <t xml:space="preserve">C2,3,6,8,9,13,15,17,22</t>
   </si>
   <si>
     <t xml:space="preserve">CC0402JRX7R6BB104</t>
@@ -245,19 +245,31 @@
     <t xml:space="preserve">311-1417-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">C14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188C81C225KA12D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2uF ceramic cap, 0603, 10%, 16V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-11993-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">C18</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM21BC80G107ME15L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100uF ceramic cap, 0805, 20%, 4V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-13978-6-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change C18 to 0805</t>
+    <t xml:space="preserve">Taiyo Yuden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMK316BC6476ML-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47uF ceramic cap, 1206, 20%, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">587-6459-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">D1,D2,D5</t>
@@ -275,12 +287,24 @@
     <t xml:space="preserve">1497-1219-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">D3,D4</t>
+    <t xml:space="preserve">D3</t>
   </si>
   <si>
     <t xml:space="preserve">Inolux</t>
   </si>
   <si>
+    <t xml:space="preserve">IN-S42BTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red LED, 0402, 2.1Vf, 20mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1830-IN-S42BCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
     <t xml:space="preserve">IN-S42BT5A</t>
   </si>
   <si>
@@ -305,12 +329,24 @@
     <t xml:space="preserve">1N4148WS-FDICT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samtec Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFM-120-01-H-D-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connector Header Through Hole, Right Angle 40 position 0.050" (1.27mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFM-120-01-H-D-RA-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">J7</t>
   </si>
   <si>
-    <t xml:space="preserve">Samtec Inc.</t>
-  </si>
-  <si>
     <t xml:space="preserve">FTSH-105-01-F-DV-K</t>
   </si>
   <si>
@@ -320,18 +356,6 @@
     <t xml:space="preserve">SAM8796-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFM-120-01-H-D-RA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector Header Through Hole, Right Angle 40 position 0.050" (1.27mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFM-120-01-H-D-RA-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">J9,10,11,12</t>
   </si>
   <si>
@@ -362,7 +386,106 @@
     <t xml:space="preserve">XC2337CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1,Q2</t>
+    <t xml:space="preserve">R1,2,3,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF2701X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2.70KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF3162X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.6k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P31.6KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF3091X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.09k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P3.09KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7,9,16,17,18,20,24,27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF1002X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10.0KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8,11,13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF4701X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P4.70KLCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-3GEY0R00V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 ohm Resistor, 0603, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0.0GCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF10R0X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10.0LCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2RKF2372X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.7k Resistor, 0402, 1%, 0.1W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P23.7KLDKR-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
   </si>
   <si>
     <t xml:space="preserve">STMicroelectronics</t>
@@ -395,12 +518,15 @@
     <t xml:space="preserve">Texas Instruments</t>
   </si>
   <si>
+    <t xml:space="preserve">TCAN330DCNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/1 Transceiver CANbus SOT-23-8</t>
+  </si>
+  <si>
     <t xml:space="preserve">296-46215-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1/1 Transceiver CANbus SOT-23-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">U4</t>
   </si>
   <si>
@@ -447,6 +573,18 @@
   </si>
   <si>
     <t xml:space="preserve">497-15376-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS-160-10-36Q-ES-TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16MHz ±30ppm Crystal 10pF 80 Ohms 4-SMD, No Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC2181CT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -1162,10 +1300,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1463,11 +1601,12 @@
       <c r="K12" s="15"/>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -1491,191 +1630,185 @@
       <c r="J13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="n">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="16" t="s">
+      <c r="F16" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="16" t="s">
+      <c r="G17" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>92</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J17" s="14" t="s">
+      <c r="I17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
     </row>
     <row r="18" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
     </row>
     <row r="19" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19" s="14" t="s">
         <v>28</v>
@@ -1689,60 +1822,60 @@
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="16" t="s">
+      <c r="G20" s="16" t="s">
         <v>104</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>106</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
     </row>
     <row r="21" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="16" t="s">
+      <c r="G21" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>111</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
@@ -1753,25 +1886,25 @@
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="15" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="G22" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>28</v>
@@ -1781,39 +1914,39 @@
     </row>
     <row r="23" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="16" t="s">
+      <c r="F23" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>120</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="15" t="s">
@@ -1823,7 +1956,7 @@
         <v>22</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>122</v>
@@ -1838,14 +1971,14 @@
         <v>124</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
     </row>
     <row r="25" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="15" t="s">
@@ -1855,7 +1988,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>126</v>
@@ -1870,14 +2003,14 @@
         <v>128</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
     </row>
     <row r="26" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
@@ -1887,7 +2020,7 @@
         <v>22</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>130</v>
@@ -1902,14 +2035,14 @@
         <v>132</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15" t="s">
@@ -1919,7 +2052,7 @@
         <v>22</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>134</v>
@@ -1934,89 +2067,427 @@
         <v>136</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14"/>
+    <row r="28" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="n">
+        <v>3</v>
+      </c>
       <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="14"/>
+      <c r="C28" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
     </row>
-    <row r="29" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="19"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="29" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+    </row>
+    <row r="30" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+    </row>
+    <row r="31" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" s="14"/>
+      <c r="C35" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+    </row>
+    <row r="37" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="14"/>
+      <c r="C37" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I37" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+    </row>
+    <row r="39" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="19"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C44" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+    <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B35" s="11" t="n">
+      <c r="B45" s="11" t="n">
         <v>43791</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" s="0" t="s">
+    <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="0" t="s">
+    <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2079,7 +2550,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -2191,7 +2662,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -2229,19 +2700,19 @@
         <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>141</v>
+        <v>187</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>28</v>
@@ -2392,7 +2863,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -2513,7 +2984,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>139</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -2551,16 +3022,16 @@
         <v>22</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>28</v>
@@ -2574,58 +3045,58 @@
         <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>151</v>
+        <v>197</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="24" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>50</v>
@@ -2639,25 +3110,25 @@
         <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>50</v>
@@ -2671,25 +3142,25 @@
         <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>50</v>
@@ -2764,7 +3235,7 @@
         <v>43738</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +3243,7 @@
         <v>43764</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2834,7 +3305,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -2850,7 +3321,7 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>216</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -3064,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Corrected part counts in the BOM
</commit_message>
<xml_diff>
--- a/BOM/C3-Practicum.xlsx
+++ b/BOM/C3-Practicum.xlsx
@@ -994,24 +994,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3705357142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1339285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,30 +1302,30 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4419642857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2053571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.65625"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,7 +1451,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0" t="s">
@@ -1481,7 +1481,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0" t="s">
@@ -1511,7 +1511,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0" t="s">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0" t="s">
@@ -1571,7 +1571,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="15" t="s">
@@ -1603,7 +1603,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="15" t="s">
@@ -1635,7 +1635,7 @@
     </row>
     <row r="14" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>73</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="0" t="s">
@@ -1694,7 +1694,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="0" t="s">
@@ -1724,7 +1724,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="0" t="s">
@@ -1754,7 +1754,7 @@
     </row>
     <row r="18" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="15" t="s">
@@ -1850,7 +1850,7 @@
     </row>
     <row r="21" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15" t="s">
@@ -1882,7 +1882,7 @@
     </row>
     <row r="22" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="15" t="s">
@@ -1914,7 +1914,7 @@
     </row>
     <row r="23" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15" t="s">
@@ -1946,7 +1946,7 @@
     </row>
     <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="15" t="s">
@@ -1978,7 +1978,7 @@
     </row>
     <row r="25" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="15" t="s">
@@ -2010,7 +2010,7 @@
     </row>
     <row r="26" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
@@ -2042,7 +2042,7 @@
     </row>
     <row r="27" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15" t="s">
@@ -2074,7 +2074,7 @@
     </row>
     <row r="28" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="15" t="s">
@@ -2106,7 +2106,7 @@
     </row>
     <row r="29" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="15" t="s">
@@ -2138,7 +2138,7 @@
     </row>
     <row r="30" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="15" t="s">
@@ -2170,7 +2170,7 @@
     </row>
     <row r="31" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="15" t="s">
@@ -2202,7 +2202,7 @@
     </row>
     <row r="32" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="15" t="s">
@@ -2234,7 +2234,7 @@
     </row>
     <row r="33" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="15" t="s">
@@ -2515,24 +2515,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,24 +2826,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0892857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="12.4017857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="16.65625"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="18" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8526785714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="12.1651785714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="16.4196428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="36.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="18" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,24 +3270,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.20535714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1205357142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.50446428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4017857142857"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3883928571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0401785714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3303571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.15178571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.7901785714286"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27.1651785714286"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.0580357142857"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0625"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.85714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7678571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added the SD card socket and changed vendors for the MAX892 on the BOM
</commit_message>
<xml_diff>
--- a/BOM/C3-Practicum.xlsx
+++ b/BOM/C3-Practicum.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="224">
   <si>
     <t xml:space="preserve">Bill Of Materials</t>
   </si>
@@ -356,6 +356,24 @@
     <t xml:space="preserve">SAM8796-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">J8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4UCON Technology Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD/MMC card Socket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparkfun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRT-12769</t>
+  </si>
+  <si>
     <t xml:space="preserve">J9,10,11,12</t>
   </si>
   <si>
@@ -509,7 +527,7 @@
     <t xml:space="preserve">Power Switch/Driver 1:1 P-Channel 250mA 8-uMAX</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX892LEUA+T-ND</t>
+    <t xml:space="preserve">700-MAX892LEUAT</t>
   </si>
   <si>
     <t xml:space="preserve">U2,U3</t>
@@ -800,7 +818,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -874,6 +892,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -994,24 +1032,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1339285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8973214285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2321428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.62053571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,32 +1338,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2053571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.65625"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.96875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.4196428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2321428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.62053571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,37 +1822,37 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="n">
+    <row r="19" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="D19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="n">
@@ -1850,7 +1888,7 @@
     </row>
     <row r="21" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15" t="s">
@@ -1869,10 +1907,10 @@
         <v>109</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>48</v>
+        <v>110</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J21" s="14" t="s">
         <v>28</v>
@@ -1882,29 +1920,29 @@
     </row>
     <row r="22" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J22" s="14" t="s">
         <v>28</v>
@@ -1914,61 +1952,61 @@
     </row>
     <row r="23" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="15" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>50</v>
@@ -1982,25 +2020,25 @@
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>50</v>
@@ -2010,29 +2048,29 @@
     </row>
     <row r="26" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="15" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J26" s="14" t="s">
         <v>50</v>
@@ -2042,29 +2080,29 @@
     </row>
     <row r="27" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>50</v>
@@ -2074,29 +2112,29 @@
     </row>
     <row r="28" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>50</v>
@@ -2106,29 +2144,29 @@
     </row>
     <row r="29" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>50</v>
@@ -2142,25 +2180,25 @@
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>50</v>
@@ -2174,25 +2212,25 @@
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>50</v>
@@ -2206,89 +2244,89 @@
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="15" t="s">
-        <v>29</v>
+        <v>155</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
     </row>
-    <row r="33" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="F33" s="16" t="s">
+    <row r="33" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="F33" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I33" s="16" t="s">
+      <c r="G33" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="H33" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
     </row>
     <row r="34" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>28</v>
@@ -2302,25 +2340,25 @@
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>28</v>
@@ -2334,25 +2372,25 @@
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>28</v>
@@ -2366,25 +2404,25 @@
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>28</v>
@@ -2392,31 +2430,31 @@
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="n">
         <v>1</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="15" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I38" s="18" t="s">
-        <v>182</v>
+      <c r="I38" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>28</v>
@@ -2424,70 +2462,102 @@
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
     </row>
-    <row r="39" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="19"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="14"/>
+      <c r="C39" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+    </row>
+    <row r="40" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
       <c r="B41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="2" t="s">
+    <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
+    <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B45" s="11" t="n">
+      <c r="B46" s="11" t="n">
         <v>43791</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C46" s="0" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="11" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C47" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2515,24 +2585,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2321428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.62053571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,7 +2620,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -2662,7 +2732,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
@@ -2700,19 +2770,19 @@
         <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>28</v>
@@ -2826,24 +2896,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8526785714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="22" width="16.4196428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="22" width="36.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="18" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="16.1830357142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="36.0267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="18" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2321428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.62053571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2863,14 +2933,14 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="27" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="0"/>
@@ -2889,7 +2959,7 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="0"/>
@@ -2951,13 +3021,13 @@
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -2984,18 +3054,18 @@
         <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -3021,17 +3091,17 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>193</v>
+      <c r="E9" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>199</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>28</v>
@@ -3045,58 +3115,58 @@
         <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>198</v>
+        <v>201</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>204</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0"/>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="G11" s="22" t="s">
-        <v>203</v>
+      <c r="F11" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>48</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>50</v>
@@ -3110,25 +3180,25 @@
         <v>20</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>208</v>
+      <c r="E12" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>214</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>50</v>
@@ -3142,25 +3212,25 @@
         <v>20</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>211</v>
+      <c r="E13" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>217</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>48</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>50</v>
@@ -3181,10 +3251,10 @@
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="9"/>
       <c r="J15" s="8"/>
       <c r="K15" s="9"/>
@@ -3235,7 +3305,7 @@
         <v>43738</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,7 +3313,7 @@
         <v>43764</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3270,24 +3340,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.08928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7678571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.38839285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1651785714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.03125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.80357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0982142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.03125"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.3169642857143"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.8125"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.5848214285714"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.74107142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.74107142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.96875"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4107142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0267857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8616071428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.5758928571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2321428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.62053571428571"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.8258928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.62053571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,7 +3375,7 @@
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -3321,7 +3391,7 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -3535,7 +3605,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>39</v>

</xml_diff>